<commit_message>
Update analysis with multiple partial models
</commit_message>
<xml_diff>
--- a/data/vars/combination.xlsx
+++ b/data/vars/combination.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="5060" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="7020" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="482">
   <si>
     <t>distance_survey_mean_1</t>
   </si>
@@ -942,268 +942,529 @@
     <t>tste_10_9</t>
   </si>
   <si>
-    <t>tste_7_0*real_extraversion</t>
-  </si>
-  <si>
-    <t>tste_7_1*real_extraversion</t>
-  </si>
-  <si>
-    <t>tste_7_2*real_extraversion</t>
-  </si>
-  <si>
-    <t>tste_7_3*real_extraversion</t>
-  </si>
-  <si>
-    <t>tste_7_4*real_extraversion</t>
-  </si>
-  <si>
-    <t>tste_7_5*real_extraversion</t>
-  </si>
-  <si>
-    <t>tste_7_6*real_extraversion</t>
-  </si>
-  <si>
-    <t>tste_7_0*real_agreeableness</t>
-  </si>
-  <si>
-    <t>tste_7_1*real_agreeableness</t>
-  </si>
-  <si>
-    <t>tste_7_2*real_agreeableness</t>
-  </si>
-  <si>
-    <t>tste_7_3*real_agreeableness</t>
-  </si>
-  <si>
-    <t>tste_7_4*real_agreeableness</t>
-  </si>
-  <si>
-    <t>tste_7_5*real_agreeableness</t>
-  </si>
-  <si>
-    <t>tste_7_6*real_agreeableness</t>
-  </si>
-  <si>
-    <t>tste_7_0*real_conscientiousness</t>
-  </si>
-  <si>
-    <t>tste_7_1*real_conscientiousness</t>
-  </si>
-  <si>
-    <t>tste_7_2*real_conscientiousness</t>
-  </si>
-  <si>
-    <t>tste_7_3*real_conscientiousness</t>
-  </si>
-  <si>
-    <t>tste_7_4*real_conscientiousness</t>
-  </si>
-  <si>
-    <t>tste_7_5*real_conscientiousness</t>
-  </si>
-  <si>
-    <t>tste_7_6*real_conscientiousness</t>
-  </si>
-  <si>
-    <t>tste_7_0*real_emotionstability</t>
-  </si>
-  <si>
-    <t>tste_7_1*real_emotionstability</t>
-  </si>
-  <si>
-    <t>tste_7_2*real_emotionstability</t>
-  </si>
-  <si>
-    <t>tste_7_3*real_emotionstability</t>
-  </si>
-  <si>
-    <t>tste_7_4*real_emotionstability</t>
-  </si>
-  <si>
-    <t>tste_7_5*real_emotionstability</t>
-  </si>
-  <si>
-    <t>tste_7_6*real_emotionstability</t>
-  </si>
-  <si>
-    <t>tste_7_0*real_openness</t>
-  </si>
-  <si>
-    <t>tste_7_1*real_openness</t>
-  </si>
-  <si>
-    <t>tste_7_2*real_openness</t>
-  </si>
-  <si>
-    <t>tste_7_3*real_openness</t>
-  </si>
-  <si>
-    <t>tste_7_4*real_openness</t>
-  </si>
-  <si>
-    <t>tste_7_5*real_openness</t>
-  </si>
-  <si>
-    <t>tste_7_6*real_openness</t>
-  </si>
-  <si>
-    <t>tste_7_0*satis_autonomy</t>
-  </si>
-  <si>
-    <t>tste_7_1*satis_autonomy</t>
-  </si>
-  <si>
-    <t>tste_7_2*satis_autonomy</t>
-  </si>
-  <si>
-    <t>tste_7_3*satis_autonomy</t>
-  </si>
-  <si>
-    <t>tste_7_4*satis_autonomy</t>
-  </si>
-  <si>
-    <t>tste_7_5*satis_autonomy</t>
-  </si>
-  <si>
-    <t>tste_7_6*satis_autonomy</t>
-  </si>
-  <si>
-    <t>tste_7_0*satis_relatedness</t>
-  </si>
-  <si>
-    <t>tste_7_1*satis_relatedness</t>
-  </si>
-  <si>
-    <t>tste_7_2*satis_relatedness</t>
-  </si>
-  <si>
-    <t>tste_7_3*satis_relatedness</t>
-  </si>
-  <si>
-    <t>tste_7_4*satis_relatedness</t>
-  </si>
-  <si>
-    <t>tste_7_5*satis_relatedness</t>
-  </si>
-  <si>
-    <t>tste_7_6*satis_relatedness</t>
-  </si>
-  <si>
-    <t>tste_7_0*satis_competence</t>
-  </si>
-  <si>
-    <t>tste_7_1*satis_competence</t>
-  </si>
-  <si>
-    <t>tste_7_2*satis_competence</t>
-  </si>
-  <si>
-    <t>tste_7_3*satis_competence</t>
-  </si>
-  <si>
-    <t>tste_7_4*satis_competence</t>
-  </si>
-  <si>
-    <t>tste_7_5*satis_competence</t>
-  </si>
-  <si>
-    <t>tste_7_6*satis_competence</t>
-  </si>
-  <si>
-    <t>tste_4_0*real_extraversion</t>
-  </si>
-  <si>
-    <t>tste_4_1*real_extraversion</t>
-  </si>
-  <si>
-    <t>tste_4_2*real_extraversion</t>
-  </si>
-  <si>
-    <t>tste_4_3*real_extraversion</t>
-  </si>
-  <si>
-    <t>tste_4_0*real_agreeableness</t>
-  </si>
-  <si>
-    <t>tste_4_1*real_agreeableness</t>
-  </si>
-  <si>
-    <t>tste_4_2*real_agreeableness</t>
-  </si>
-  <si>
-    <t>tste_4_3*real_agreeableness</t>
-  </si>
-  <si>
-    <t>tste_4_0*real_conscientiousness</t>
-  </si>
-  <si>
-    <t>tste_4_1*real_conscientiousness</t>
-  </si>
-  <si>
-    <t>tste_4_2*real_conscientiousness</t>
-  </si>
-  <si>
-    <t>tste_4_3*real_conscientiousness</t>
-  </si>
-  <si>
-    <t>tste_4_0*real_emotionstability</t>
-  </si>
-  <si>
-    <t>tste_4_1*real_emotionstability</t>
-  </si>
-  <si>
-    <t>tste_4_2*real_emotionstability</t>
-  </si>
-  <si>
-    <t>tste_4_3*real_emotionstability</t>
-  </si>
-  <si>
-    <t>tste_4_0*real_openness</t>
-  </si>
-  <si>
-    <t>tste_4_1*real_openness</t>
-  </si>
-  <si>
-    <t>tste_4_2*real_openness</t>
-  </si>
-  <si>
-    <t>tste_4_3*real_openness</t>
-  </si>
-  <si>
-    <t>tste_4_0*satis_autonomy</t>
-  </si>
-  <si>
-    <t>tste_4_1*satis_autonomy</t>
-  </si>
-  <si>
-    <t>tste_4_2*satis_autonomy</t>
-  </si>
-  <si>
-    <t>tste_4_3*satis_autonomy</t>
-  </si>
-  <si>
-    <t>tste_4_0*satis_relatedness</t>
-  </si>
-  <si>
-    <t>tste_4_1*satis_relatedness</t>
-  </si>
-  <si>
-    <t>tste_4_2*satis_relatedness</t>
-  </si>
-  <si>
-    <t>tste_4_3*satis_relatedness</t>
-  </si>
-  <si>
-    <t>tste_4_0*satis_competence</t>
-  </si>
-  <si>
-    <t>tste_4_1*satis_competence</t>
-  </si>
-  <si>
-    <t>tste_4_2*satis_competence</t>
-  </si>
-  <si>
-    <t>tste_4_3*satis_competence</t>
+    <t>tste_4_0*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_4_1*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_4_2*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_4_3*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_4_0*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_4_1*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_4_2*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_4_3*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_4_0*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_4_1*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_4_2*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_4_3*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_4_0*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_4_1*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_4_2*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_4_3*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_4_0*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_4_1*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_4_2*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_4_3*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_8_0*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_8_1*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_8_2*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_8_3*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_8_4*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_8_5*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_8_6*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_8_7*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_8_0*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_8_1*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_8_2*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_8_3*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_8_4*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_8_5*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_8_6*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_8_7*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_8_0*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_8_1*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_8_2*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_8_3*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_8_4*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_8_5*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_8_6*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_8_7*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_8_0*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_8_1*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_8_2*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_8_3*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_8_4*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_8_5*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_8_6*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_8_7*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_8_0*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_8_1*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_8_2*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_8_3*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_8_4*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_8_5*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_8_6*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_8_7*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_5_0*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_5_1*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_5_2*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_5_3*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_5_4*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_5_0*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_5_1*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_5_2*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_5_3*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_5_4*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_5_0*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_5_1*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_5_2*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_5_3*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_5_4*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_5_0*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_5_1*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_5_2*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_5_3*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_5_4*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_5_0*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_5_1*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_5_2*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_5_3*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_5_4*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_3_0*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_3_1*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_3_2*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_3_0*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_3_1*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_3_2*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_3_0*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_3_1*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_3_2*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_3_0*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_3_1*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_3_2*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_3_0*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_3_1*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_3_2*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_6_0*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_6_1*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_6_2*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_6_3*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_6_4*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_6_5*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_6_0*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_6_1*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_6_2*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_6_3*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_6_4*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_6_5*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_6_0*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_6_1*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_6_2*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_6_3*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_6_4*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_6_5*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_6_0*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_6_1*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_6_2*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_6_3*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_6_4*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_6_5*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_6_0*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_6_1*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_6_2*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_6_3*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_6_4*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_6_5*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_7_0*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_7_1*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_7_2*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_7_3*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_7_4*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_7_5*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_7_6*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_7_0*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_7_1*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_7_2*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_7_3*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_7_4*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_7_5*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_7_6*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_7_0*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_7_1*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_7_2*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_7_3*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_7_4*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_7_5*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_7_6*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_7_0*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_7_1*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_7_2*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_7_3*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_7_4*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_7_5*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_7_6*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_7_0*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_7_1*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_7_2*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_7_3*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_7_4*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_7_5*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_7_6*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_2_0*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_2_1*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_2_0*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_2_1*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_2_0*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_2_1*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_2_0*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_2_1*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_2_0*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_2_1*gap_openness</t>
   </si>
 </sst>
 </file>
@@ -1528,10 +1789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q116"/>
+  <dimension ref="A1:V116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="S4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X23" sqref="X23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1543,10 +1804,13 @@
     <col min="11" max="11" width="32.81640625" customWidth="1"/>
     <col min="12" max="12" width="45.1796875" customWidth="1"/>
     <col min="13" max="15" width="45.08984375" customWidth="1"/>
-    <col min="16" max="17" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.453125" customWidth="1"/>
+    <col min="18" max="21" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="28.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1575,13 +1839,28 @@
         <v>181</v>
       </c>
       <c r="P1" t="s">
-        <v>181</v>
+        <v>12</v>
       </c>
       <c r="Q1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="R1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T1" t="s">
+        <v>12</v>
+      </c>
+      <c r="U1" t="s">
+        <v>12</v>
+      </c>
+      <c r="V1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1615,8 +1894,23 @@
       <c r="Q2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R2" t="s">
+        <v>13</v>
+      </c>
+      <c r="S2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T2" t="s">
+        <v>13</v>
+      </c>
+      <c r="U2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1650,8 +1944,23 @@
       <c r="Q3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S3" t="s">
+        <v>14</v>
+      </c>
+      <c r="T3" t="s">
+        <v>14</v>
+      </c>
+      <c r="U3" t="s">
+        <v>14</v>
+      </c>
+      <c r="V3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1677,13 +1986,28 @@
         <v>17</v>
       </c>
       <c r="P4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="Q4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+      <c r="R4" t="s">
+        <v>15</v>
+      </c>
+      <c r="S4" t="s">
+        <v>15</v>
+      </c>
+      <c r="T4" t="s">
+        <v>15</v>
+      </c>
+      <c r="U4" t="s">
+        <v>15</v>
+      </c>
+      <c r="V4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1709,13 +2033,28 @@
         <v>7</v>
       </c>
       <c r="P5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Q5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="R5" t="s">
+        <v>16</v>
+      </c>
+      <c r="S5" t="s">
+        <v>16</v>
+      </c>
+      <c r="T5" t="s">
+        <v>16</v>
+      </c>
+      <c r="U5" t="s">
+        <v>16</v>
+      </c>
+      <c r="V5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1744,13 +2083,28 @@
         <v>8</v>
       </c>
       <c r="P6" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="Q6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+      <c r="R6" t="s">
+        <v>17</v>
+      </c>
+      <c r="S6" t="s">
+        <v>17</v>
+      </c>
+      <c r="T6" t="s">
+        <v>17</v>
+      </c>
+      <c r="U6" t="s">
+        <v>17</v>
+      </c>
+      <c r="V6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1779,13 +2133,28 @@
         <v>9</v>
       </c>
       <c r="P7" t="s">
-        <v>9</v>
+        <v>181</v>
       </c>
       <c r="Q7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+        <v>181</v>
+      </c>
+      <c r="R7" t="s">
+        <v>181</v>
+      </c>
+      <c r="S7" t="s">
+        <v>181</v>
+      </c>
+      <c r="T7" t="s">
+        <v>181</v>
+      </c>
+      <c r="U7" t="s">
+        <v>181</v>
+      </c>
+      <c r="V7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>181</v>
       </c>
@@ -1814,13 +2183,28 @@
         <v>10</v>
       </c>
       <c r="P8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="Q8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="R8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S8" t="s">
+        <v>7</v>
+      </c>
+      <c r="T8" t="s">
+        <v>7</v>
+      </c>
+      <c r="U8" t="s">
+        <v>7</v>
+      </c>
+      <c r="V8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1849,13 +2233,28 @@
         <v>11</v>
       </c>
       <c r="P9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="Q9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="R9" t="s">
+        <v>8</v>
+      </c>
+      <c r="S9" t="s">
+        <v>8</v>
+      </c>
+      <c r="T9" t="s">
+        <v>8</v>
+      </c>
+      <c r="U9" t="s">
+        <v>8</v>
+      </c>
+      <c r="V9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1884,13 +2283,28 @@
         <v>64</v>
       </c>
       <c r="P10" t="s">
-        <v>273</v>
+        <v>9</v>
       </c>
       <c r="Q10" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="R10" t="s">
+        <v>9</v>
+      </c>
+      <c r="S10" t="s">
+        <v>9</v>
+      </c>
+      <c r="T10" t="s">
+        <v>9</v>
+      </c>
+      <c r="U10" t="s">
+        <v>9</v>
+      </c>
+      <c r="V10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1916,13 +2330,28 @@
         <v>65</v>
       </c>
       <c r="P11" t="s">
-        <v>274</v>
+        <v>10</v>
       </c>
       <c r="Q11" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="R11" t="s">
+        <v>10</v>
+      </c>
+      <c r="S11" t="s">
+        <v>10</v>
+      </c>
+      <c r="T11" t="s">
+        <v>10</v>
+      </c>
+      <c r="U11" t="s">
+        <v>10</v>
+      </c>
+      <c r="V11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1945,13 +2374,28 @@
         <v>66</v>
       </c>
       <c r="P12" t="s">
-        <v>275</v>
+        <v>11</v>
       </c>
       <c r="Q12" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+      <c r="R12" t="s">
+        <v>11</v>
+      </c>
+      <c r="S12" t="s">
+        <v>11</v>
+      </c>
+      <c r="T12" t="s">
+        <v>11</v>
+      </c>
+      <c r="U12" t="s">
+        <v>11</v>
+      </c>
+      <c r="V12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1974,13 +2418,28 @@
         <v>238</v>
       </c>
       <c r="P13" t="s">
-        <v>276</v>
+        <v>59</v>
       </c>
       <c r="Q13" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+      <c r="R13" t="s">
+        <v>59</v>
+      </c>
+      <c r="S13" t="s">
+        <v>59</v>
+      </c>
+      <c r="T13" t="s">
+        <v>59</v>
+      </c>
+      <c r="U13" t="s">
+        <v>59</v>
+      </c>
+      <c r="V13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -2003,13 +2462,28 @@
         <v>239</v>
       </c>
       <c r="P14" t="s">
-        <v>277</v>
+        <v>60</v>
       </c>
       <c r="Q14" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+      <c r="R14" t="s">
+        <v>60</v>
+      </c>
+      <c r="S14" t="s">
+        <v>60</v>
+      </c>
+      <c r="T14" t="s">
+        <v>60</v>
+      </c>
+      <c r="U14" t="s">
+        <v>60</v>
+      </c>
+      <c r="V14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -2032,13 +2506,28 @@
         <v>240</v>
       </c>
       <c r="P15" t="s">
-        <v>278</v>
+        <v>61</v>
       </c>
       <c r="Q15" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+      <c r="R15" t="s">
+        <v>61</v>
+      </c>
+      <c r="S15" t="s">
+        <v>61</v>
+      </c>
+      <c r="T15" t="s">
+        <v>61</v>
+      </c>
+      <c r="U15" t="s">
+        <v>61</v>
+      </c>
+      <c r="V15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -2061,13 +2550,28 @@
         <v>241</v>
       </c>
       <c r="P16" t="s">
-        <v>279</v>
+        <v>62</v>
       </c>
       <c r="Q16" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+      <c r="R16" t="s">
+        <v>62</v>
+      </c>
+      <c r="S16" t="s">
+        <v>62</v>
+      </c>
+      <c r="T16" t="s">
+        <v>62</v>
+      </c>
+      <c r="U16" t="s">
+        <v>62</v>
+      </c>
+      <c r="V16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -2090,13 +2594,28 @@
         <v>242</v>
       </c>
       <c r="P17" t="s">
-        <v>307</v>
+        <v>63</v>
       </c>
       <c r="Q17" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="R17" t="s">
+        <v>63</v>
+      </c>
+      <c r="S17" t="s">
+        <v>63</v>
+      </c>
+      <c r="T17" t="s">
+        <v>63</v>
+      </c>
+      <c r="U17" t="s">
+        <v>63</v>
+      </c>
+      <c r="V17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -2119,13 +2638,28 @@
         <v>243</v>
       </c>
       <c r="P18" t="s">
-        <v>308</v>
+        <v>253</v>
       </c>
       <c r="Q18" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+        <v>255</v>
+      </c>
+      <c r="R18" t="s">
+        <v>258</v>
+      </c>
+      <c r="S18" t="s">
+        <v>262</v>
+      </c>
+      <c r="T18" t="s">
+        <v>267</v>
+      </c>
+      <c r="U18" t="s">
+        <v>273</v>
+      </c>
+      <c r="V18" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -2148,13 +2682,28 @@
         <v>244</v>
       </c>
       <c r="P19" t="s">
-        <v>309</v>
+        <v>254</v>
       </c>
       <c r="Q19" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+        <v>256</v>
+      </c>
+      <c r="R19" t="s">
+        <v>259</v>
+      </c>
+      <c r="S19" t="s">
+        <v>263</v>
+      </c>
+      <c r="T19" t="s">
+        <v>268</v>
+      </c>
+      <c r="U19" t="s">
+        <v>274</v>
+      </c>
+      <c r="V19" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -2177,13 +2726,28 @@
         <v>245</v>
       </c>
       <c r="P20" t="s">
-        <v>310</v>
+        <v>472</v>
       </c>
       <c r="Q20" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+        <v>257</v>
+      </c>
+      <c r="R20" t="s">
+        <v>260</v>
+      </c>
+      <c r="S20" t="s">
+        <v>264</v>
+      </c>
+      <c r="T20" t="s">
+        <v>269</v>
+      </c>
+      <c r="U20" t="s">
+        <v>275</v>
+      </c>
+      <c r="V20" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -2206,13 +2770,28 @@
         <v>246</v>
       </c>
       <c r="P21" t="s">
-        <v>311</v>
+        <v>473</v>
       </c>
       <c r="Q21" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+        <v>392</v>
+      </c>
+      <c r="R21" t="s">
+        <v>261</v>
+      </c>
+      <c r="S21" t="s">
+        <v>265</v>
+      </c>
+      <c r="T21" t="s">
+        <v>270</v>
+      </c>
+      <c r="U21" t="s">
+        <v>276</v>
+      </c>
+      <c r="V21" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -2232,13 +2811,28 @@
         <v>247</v>
       </c>
       <c r="P22" t="s">
-        <v>312</v>
+        <v>474</v>
       </c>
       <c r="Q22" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+        <v>393</v>
+      </c>
+      <c r="R22" t="s">
+        <v>307</v>
+      </c>
+      <c r="S22" t="s">
+        <v>266</v>
+      </c>
+      <c r="T22" t="s">
+        <v>271</v>
+      </c>
+      <c r="U22" t="s">
+        <v>277</v>
+      </c>
+      <c r="V22" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -2258,13 +2852,28 @@
         <v>248</v>
       </c>
       <c r="P23" t="s">
-        <v>313</v>
+        <v>475</v>
       </c>
       <c r="Q23" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+        <v>394</v>
+      </c>
+      <c r="R23" t="s">
+        <v>308</v>
+      </c>
+      <c r="S23" t="s">
+        <v>367</v>
+      </c>
+      <c r="T23" t="s">
+        <v>272</v>
+      </c>
+      <c r="U23" t="s">
+        <v>278</v>
+      </c>
+      <c r="V23" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -2284,13 +2893,28 @@
         <v>249</v>
       </c>
       <c r="P24" t="s">
-        <v>314</v>
+        <v>476</v>
       </c>
       <c r="Q24" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+        <v>395</v>
+      </c>
+      <c r="R24" t="s">
+        <v>309</v>
+      </c>
+      <c r="S24" t="s">
+        <v>368</v>
+      </c>
+      <c r="T24" t="s">
+        <v>407</v>
+      </c>
+      <c r="U24" t="s">
+        <v>279</v>
+      </c>
+      <c r="V24" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>65</v>
       </c>
@@ -2310,13 +2934,28 @@
         <v>250</v>
       </c>
       <c r="P25" t="s">
-        <v>315</v>
+        <v>477</v>
       </c>
       <c r="Q25" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+        <v>396</v>
+      </c>
+      <c r="R25" t="s">
+        <v>310</v>
+      </c>
+      <c r="S25" t="s">
+        <v>369</v>
+      </c>
+      <c r="T25" t="s">
+        <v>408</v>
+      </c>
+      <c r="U25" t="s">
+        <v>437</v>
+      </c>
+      <c r="V25" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -2336,13 +2975,28 @@
         <v>251</v>
       </c>
       <c r="P26" t="s">
-        <v>316</v>
+        <v>478</v>
       </c>
       <c r="Q26" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+        <v>397</v>
+      </c>
+      <c r="R26" t="s">
+        <v>311</v>
+      </c>
+      <c r="S26" t="s">
+        <v>370</v>
+      </c>
+      <c r="T26" t="s">
+        <v>409</v>
+      </c>
+      <c r="U26" t="s">
+        <v>438</v>
+      </c>
+      <c r="V26" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -2362,13 +3016,28 @@
         <v>252</v>
       </c>
       <c r="P27" t="s">
-        <v>317</v>
+        <v>479</v>
       </c>
       <c r="Q27" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+        <v>398</v>
+      </c>
+      <c r="R27" t="s">
+        <v>312</v>
+      </c>
+      <c r="S27" t="s">
+        <v>371</v>
+      </c>
+      <c r="T27" t="s">
+        <v>410</v>
+      </c>
+      <c r="U27" t="s">
+        <v>439</v>
+      </c>
+      <c r="V27" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>68</v>
       </c>
@@ -2385,13 +3054,28 @@
         <v>192</v>
       </c>
       <c r="P28" t="s">
-        <v>318</v>
+        <v>480</v>
       </c>
       <c r="Q28" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+        <v>399</v>
+      </c>
+      <c r="R28" t="s">
+        <v>313</v>
+      </c>
+      <c r="S28" t="s">
+        <v>372</v>
+      </c>
+      <c r="T28" t="s">
+        <v>411</v>
+      </c>
+      <c r="U28" t="s">
+        <v>440</v>
+      </c>
+      <c r="V28" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -2408,13 +3092,28 @@
         <v>193</v>
       </c>
       <c r="P29" t="s">
-        <v>319</v>
+        <v>481</v>
       </c>
       <c r="Q29" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+        <v>400</v>
+      </c>
+      <c r="R29" t="s">
+        <v>314</v>
+      </c>
+      <c r="S29" t="s">
+        <v>373</v>
+      </c>
+      <c r="T29" t="s">
+        <v>412</v>
+      </c>
+      <c r="U29" t="s">
+        <v>441</v>
+      </c>
+      <c r="V29" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>70</v>
       </c>
@@ -2430,14 +3129,26 @@
       <c r="N30" t="s">
         <v>194</v>
       </c>
-      <c r="P30" t="s">
-        <v>320</v>
-      </c>
       <c r="Q30" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+        <v>401</v>
+      </c>
+      <c r="R30" t="s">
+        <v>315</v>
+      </c>
+      <c r="S30" t="s">
+        <v>374</v>
+      </c>
+      <c r="T30" t="s">
+        <v>413</v>
+      </c>
+      <c r="U30" t="s">
+        <v>442</v>
+      </c>
+      <c r="V30" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>71</v>
       </c>
@@ -2453,14 +3164,26 @@
       <c r="N31" t="s">
         <v>195</v>
       </c>
-      <c r="P31" t="s">
-        <v>321</v>
-      </c>
       <c r="Q31" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+        <v>402</v>
+      </c>
+      <c r="R31" t="s">
+        <v>316</v>
+      </c>
+      <c r="S31" t="s">
+        <v>375</v>
+      </c>
+      <c r="T31" t="s">
+        <v>414</v>
+      </c>
+      <c r="U31" t="s">
+        <v>443</v>
+      </c>
+      <c r="V31" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>72</v>
       </c>
@@ -2476,14 +3199,26 @@
       <c r="N32" t="s">
         <v>196</v>
       </c>
-      <c r="P32" t="s">
-        <v>322</v>
-      </c>
       <c r="Q32" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+        <v>403</v>
+      </c>
+      <c r="R32" t="s">
+        <v>317</v>
+      </c>
+      <c r="S32" t="s">
+        <v>376</v>
+      </c>
+      <c r="T32" t="s">
+        <v>415</v>
+      </c>
+      <c r="U32" t="s">
+        <v>444</v>
+      </c>
+      <c r="V32" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -2499,14 +3234,26 @@
       <c r="N33" t="s">
         <v>197</v>
       </c>
-      <c r="P33" t="s">
-        <v>323</v>
-      </c>
       <c r="Q33" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+        <v>404</v>
+      </c>
+      <c r="R33" t="s">
+        <v>318</v>
+      </c>
+      <c r="S33" t="s">
+        <v>377</v>
+      </c>
+      <c r="T33" t="s">
+        <v>416</v>
+      </c>
+      <c r="U33" t="s">
+        <v>445</v>
+      </c>
+      <c r="V33" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -2522,14 +3269,26 @@
       <c r="N34" t="s">
         <v>198</v>
       </c>
-      <c r="P34" t="s">
-        <v>324</v>
-      </c>
       <c r="Q34" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+        <v>405</v>
+      </c>
+      <c r="R34" t="s">
+        <v>319</v>
+      </c>
+      <c r="S34" t="s">
+        <v>378</v>
+      </c>
+      <c r="T34" t="s">
+        <v>417</v>
+      </c>
+      <c r="U34" t="s">
+        <v>446</v>
+      </c>
+      <c r="V34" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -2545,14 +3304,26 @@
       <c r="N35" t="s">
         <v>199</v>
       </c>
-      <c r="P35" t="s">
-        <v>325</v>
-      </c>
       <c r="Q35" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+        <v>406</v>
+      </c>
+      <c r="R35" t="s">
+        <v>320</v>
+      </c>
+      <c r="S35" t="s">
+        <v>379</v>
+      </c>
+      <c r="T35" t="s">
+        <v>418</v>
+      </c>
+      <c r="U35" t="s">
+        <v>447</v>
+      </c>
+      <c r="V35" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>3</v>
       </c>
@@ -2565,14 +3336,23 @@
       <c r="N36" t="s">
         <v>200</v>
       </c>
-      <c r="P36" t="s">
-        <v>326</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R36" t="s">
+        <v>321</v>
+      </c>
+      <c r="S36" t="s">
+        <v>380</v>
+      </c>
+      <c r="T36" t="s">
+        <v>419</v>
+      </c>
+      <c r="U36" t="s">
+        <v>448</v>
+      </c>
+      <c r="V36" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -2585,14 +3365,23 @@
       <c r="N37" t="s">
         <v>201</v>
       </c>
-      <c r="P37" t="s">
-        <v>327</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R37" t="s">
+        <v>322</v>
+      </c>
+      <c r="S37" t="s">
+        <v>381</v>
+      </c>
+      <c r="T37" t="s">
+        <v>420</v>
+      </c>
+      <c r="U37" t="s">
+        <v>449</v>
+      </c>
+      <c r="V37" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -2605,14 +3394,23 @@
       <c r="N38" t="s">
         <v>202</v>
       </c>
-      <c r="P38" t="s">
-        <v>328</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R38" t="s">
+        <v>323</v>
+      </c>
+      <c r="S38" t="s">
+        <v>382</v>
+      </c>
+      <c r="T38" t="s">
+        <v>421</v>
+      </c>
+      <c r="U38" t="s">
+        <v>450</v>
+      </c>
+      <c r="V38" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -2625,14 +3423,23 @@
       <c r="N39" t="s">
         <v>203</v>
       </c>
-      <c r="P39" t="s">
-        <v>329</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R39" t="s">
+        <v>324</v>
+      </c>
+      <c r="S39" t="s">
+        <v>383</v>
+      </c>
+      <c r="T39" t="s">
+        <v>422</v>
+      </c>
+      <c r="U39" t="s">
+        <v>451</v>
+      </c>
+      <c r="V39" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>75</v>
       </c>
@@ -2645,14 +3452,23 @@
       <c r="N40" t="s">
         <v>204</v>
       </c>
-      <c r="P40" t="s">
-        <v>330</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R40" t="s">
+        <v>325</v>
+      </c>
+      <c r="S40" t="s">
+        <v>384</v>
+      </c>
+      <c r="T40" t="s">
+        <v>423</v>
+      </c>
+      <c r="U40" t="s">
+        <v>452</v>
+      </c>
+      <c r="V40" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>76</v>
       </c>
@@ -2665,14 +3481,23 @@
       <c r="N41" t="s">
         <v>205</v>
       </c>
-      <c r="P41" t="s">
-        <v>331</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R41" t="s">
+        <v>326</v>
+      </c>
+      <c r="S41" t="s">
+        <v>385</v>
+      </c>
+      <c r="T41" t="s">
+        <v>424</v>
+      </c>
+      <c r="U41" t="s">
+        <v>453</v>
+      </c>
+      <c r="V41" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>77</v>
       </c>
@@ -2685,14 +3510,20 @@
       <c r="N42" t="s">
         <v>206</v>
       </c>
-      <c r="P42" t="s">
-        <v>332</v>
-      </c>
-      <c r="Q42" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S42" t="s">
+        <v>386</v>
+      </c>
+      <c r="T42" t="s">
+        <v>425</v>
+      </c>
+      <c r="U42" t="s">
+        <v>454</v>
+      </c>
+      <c r="V42" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>78</v>
       </c>
@@ -2705,14 +3536,20 @@
       <c r="N43" t="s">
         <v>207</v>
       </c>
-      <c r="P43" t="s">
-        <v>333</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S43" t="s">
+        <v>387</v>
+      </c>
+      <c r="T43" t="s">
+        <v>426</v>
+      </c>
+      <c r="U43" t="s">
+        <v>455</v>
+      </c>
+      <c r="V43" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>79</v>
       </c>
@@ -2725,14 +3562,20 @@
       <c r="N44" t="s">
         <v>208</v>
       </c>
-      <c r="P44" t="s">
-        <v>334</v>
-      </c>
-      <c r="Q44" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S44" t="s">
+        <v>388</v>
+      </c>
+      <c r="T44" t="s">
+        <v>427</v>
+      </c>
+      <c r="U44" t="s">
+        <v>456</v>
+      </c>
+      <c r="V44" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>80</v>
       </c>
@@ -2745,14 +3588,20 @@
       <c r="N45" t="s">
         <v>209</v>
       </c>
-      <c r="P45" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q45" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S45" t="s">
+        <v>389</v>
+      </c>
+      <c r="T45" t="s">
+        <v>428</v>
+      </c>
+      <c r="U45" t="s">
+        <v>457</v>
+      </c>
+      <c r="V45" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>81</v>
       </c>
@@ -2765,14 +3614,20 @@
       <c r="N46" t="s">
         <v>210</v>
       </c>
-      <c r="P46" t="s">
-        <v>336</v>
-      </c>
-      <c r="Q46" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S46" t="s">
+        <v>390</v>
+      </c>
+      <c r="T46" t="s">
+        <v>429</v>
+      </c>
+      <c r="U46" t="s">
+        <v>458</v>
+      </c>
+      <c r="V46" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>82</v>
       </c>
@@ -2785,14 +3640,20 @@
       <c r="N47" t="s">
         <v>211</v>
       </c>
-      <c r="P47" t="s">
-        <v>337</v>
-      </c>
-      <c r="Q47" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S47" t="s">
+        <v>391</v>
+      </c>
+      <c r="T47" t="s">
+        <v>430</v>
+      </c>
+      <c r="U47" t="s">
+        <v>459</v>
+      </c>
+      <c r="V47" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>83</v>
       </c>
@@ -2805,14 +3666,17 @@
       <c r="N48" t="s">
         <v>212</v>
       </c>
-      <c r="P48" t="s">
-        <v>338</v>
-      </c>
-      <c r="Q48" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="T48" t="s">
+        <v>431</v>
+      </c>
+      <c r="U48" t="s">
+        <v>460</v>
+      </c>
+      <c r="V48" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>84</v>
       </c>
@@ -2825,11 +3689,17 @@
       <c r="N49" t="s">
         <v>213</v>
       </c>
-      <c r="P49" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="T49" t="s">
+        <v>432</v>
+      </c>
+      <c r="U49" t="s">
+        <v>461</v>
+      </c>
+      <c r="V49" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>85</v>
       </c>
@@ -2842,11 +3712,17 @@
       <c r="N50" t="s">
         <v>214</v>
       </c>
-      <c r="P50" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="T50" t="s">
+        <v>433</v>
+      </c>
+      <c r="U50" t="s">
+        <v>462</v>
+      </c>
+      <c r="V50" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>86</v>
       </c>
@@ -2859,11 +3735,17 @@
       <c r="N51" t="s">
         <v>215</v>
       </c>
-      <c r="P51" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="T51" t="s">
+        <v>434</v>
+      </c>
+      <c r="U51" t="s">
+        <v>463</v>
+      </c>
+      <c r="V51" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>87</v>
       </c>
@@ -2873,11 +3755,17 @@
       <c r="N52" t="s">
         <v>216</v>
       </c>
-      <c r="P52" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="T52" t="s">
+        <v>435</v>
+      </c>
+      <c r="U52" t="s">
+        <v>464</v>
+      </c>
+      <c r="V52" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>88</v>
       </c>
@@ -2887,11 +3775,17 @@
       <c r="N53" t="s">
         <v>70</v>
       </c>
-      <c r="P53" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="T53" t="s">
+        <v>436</v>
+      </c>
+      <c r="U53" t="s">
+        <v>465</v>
+      </c>
+      <c r="V53" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>89</v>
       </c>
@@ -2901,11 +3795,14 @@
       <c r="N54" t="s">
         <v>71</v>
       </c>
-      <c r="P54" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="U54" t="s">
+        <v>466</v>
+      </c>
+      <c r="V54" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>90</v>
       </c>
@@ -2915,11 +3812,14 @@
       <c r="N55" t="s">
         <v>72</v>
       </c>
-      <c r="P55" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="U55" t="s">
+        <v>467</v>
+      </c>
+      <c r="V55" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>91</v>
       </c>
@@ -2929,11 +3829,14 @@
       <c r="N56" t="s">
         <v>217</v>
       </c>
-      <c r="P56" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="U56" t="s">
+        <v>468</v>
+      </c>
+      <c r="V56" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>92</v>
       </c>
@@ -2943,11 +3846,14 @@
       <c r="N57" t="s">
         <v>218</v>
       </c>
-      <c r="P57" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="U57" t="s">
+        <v>469</v>
+      </c>
+      <c r="V57" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>93</v>
       </c>
@@ -2957,11 +3863,14 @@
       <c r="N58" t="s">
         <v>219</v>
       </c>
-      <c r="P58" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="U58" t="s">
+        <v>470</v>
+      </c>
+      <c r="V58" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>94</v>
       </c>
@@ -2971,11 +3880,14 @@
       <c r="N59" t="s">
         <v>220</v>
       </c>
-      <c r="P59" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="U59" t="s">
+        <v>471</v>
+      </c>
+      <c r="V59" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>95</v>
       </c>
@@ -2985,11 +3897,11 @@
       <c r="N60" t="s">
         <v>221</v>
       </c>
-      <c r="P60" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="V60" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>73</v>
       </c>
@@ -2999,11 +3911,11 @@
       <c r="N61" t="s">
         <v>222</v>
       </c>
-      <c r="P61" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="V61" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>74</v>
       </c>
@@ -3013,11 +3925,11 @@
       <c r="N62" t="s">
         <v>223</v>
       </c>
-      <c r="P62" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="V62" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>253</v>
       </c>
@@ -3027,11 +3939,11 @@
       <c r="N63" t="s">
         <v>224</v>
       </c>
-      <c r="P63" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="V63" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>254</v>
       </c>
@@ -3041,11 +3953,11 @@
       <c r="N64" t="s">
         <v>225</v>
       </c>
-      <c r="P64" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="V64" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>255</v>
       </c>
@@ -3055,11 +3967,11 @@
       <c r="N65" t="s">
         <v>226</v>
       </c>
-      <c r="P65" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="V65" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>256</v>
       </c>
@@ -3069,11 +3981,8 @@
       <c r="N66" t="s">
         <v>227</v>
       </c>
-      <c r="P66" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="67" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>257</v>
       </c>
@@ -3083,11 +3992,8 @@
       <c r="N67" t="s">
         <v>228</v>
       </c>
-      <c r="P67" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="68" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>258</v>
       </c>
@@ -3097,11 +4003,8 @@
       <c r="N68" t="s">
         <v>229</v>
       </c>
-      <c r="P68" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="69" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>259</v>
       </c>
@@ -3111,11 +4014,8 @@
       <c r="N69" t="s">
         <v>230</v>
       </c>
-      <c r="P69" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>260</v>
       </c>
@@ -3125,11 +4025,8 @@
       <c r="N70" t="s">
         <v>231</v>
       </c>
-      <c r="P70" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="71" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>261</v>
       </c>
@@ -3139,11 +4036,8 @@
       <c r="N71" t="s">
         <v>232</v>
       </c>
-      <c r="P71" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="72" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>262</v>
       </c>
@@ -3153,11 +4047,8 @@
       <c r="N72" t="s">
         <v>233</v>
       </c>
-      <c r="P72" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="73" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>263</v>
       </c>
@@ -3167,11 +4058,8 @@
       <c r="N73" t="s">
         <v>234</v>
       </c>
-      <c r="P73" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>264</v>
       </c>
@@ -3181,11 +4069,8 @@
       <c r="N74" t="s">
         <v>235</v>
       </c>
-      <c r="P74" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>265</v>
       </c>
@@ -3195,11 +4080,8 @@
       <c r="N75" t="s">
         <v>236</v>
       </c>
-      <c r="P75" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="76" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>266</v>
       </c>
@@ -3207,22 +4089,22 @@
         <v>237</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>270</v>
       </c>

</xml_diff>

<commit_message>
Prepare for adding new analysis
</commit_message>
<xml_diff>
--- a/data/vars/combination.xlsx
+++ b/data/vars/combination.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="7020" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="8980" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="689">
   <si>
     <t>distance_survey_mean_1</t>
   </si>
@@ -1465,6 +1465,627 @@
   </si>
   <si>
     <t>tste_2_1*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_9_0*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_9_1*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_9_2*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_9_3*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_9_4*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_9_5*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_9_6*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_9_7*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_9_0*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_9_1*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_9_2*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_9_3*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_9_4*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_9_5*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_9_6*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_9_7*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_9_0*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_9_1*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_9_2*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_9_3*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_9_4*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_9_5*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_9_6*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_9_7*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_9_0*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_9_1*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_9_2*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_9_3*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_9_4*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_9_5*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_9_6*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_9_7*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_9_0*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_9_1*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_9_2*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_9_3*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_9_4*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_9_5*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_9_6*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_9_7*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_9_8*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_9_8*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_9_8*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_9_8*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_9_8*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_11_0</t>
+  </si>
+  <si>
+    <t>tste_11_1</t>
+  </si>
+  <si>
+    <t>tste_11_2</t>
+  </si>
+  <si>
+    <t>tste_11_3</t>
+  </si>
+  <si>
+    <t>tste_11_4</t>
+  </si>
+  <si>
+    <t>tste_11_5</t>
+  </si>
+  <si>
+    <t>tste_11_6</t>
+  </si>
+  <si>
+    <t>tste_11_7</t>
+  </si>
+  <si>
+    <t>tste_11_8</t>
+  </si>
+  <si>
+    <t>tste_11_9</t>
+  </si>
+  <si>
+    <t>tste_11_10</t>
+  </si>
+  <si>
+    <t>tste_11_0*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_11_1*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_11_2*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_11_3*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_11_4*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_11_5*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_11_6*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_11_7*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_11_8*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_11_9*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_11_10*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_11_0*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_11_1*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_11_2*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_11_3*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_11_4*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_11_5*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_11_6*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_11_7*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_11_8*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_11_9*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_11_10*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_11_0*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_11_1*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_11_2*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_11_3*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_11_4*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_11_5*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_11_6*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_11_7*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_11_8*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_11_9*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_11_10*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_11_0*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_11_1*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_11_2*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_11_3*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_11_4*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_11_5*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_11_6*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_11_7*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_11_8*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_11_9*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_11_10*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_11_0*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_11_1*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_11_2*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_11_3*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_11_4*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_11_5*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_11_6*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_11_7*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_11_8*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_11_9*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_11_10*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_16_0</t>
+  </si>
+  <si>
+    <t>tste_16_1</t>
+  </si>
+  <si>
+    <t>tste_16_2</t>
+  </si>
+  <si>
+    <t>tste_16_3</t>
+  </si>
+  <si>
+    <t>tste_16_4</t>
+  </si>
+  <si>
+    <t>tste_16_5</t>
+  </si>
+  <si>
+    <t>tste_16_6</t>
+  </si>
+  <si>
+    <t>tste_16_7</t>
+  </si>
+  <si>
+    <t>tste_16_8</t>
+  </si>
+  <si>
+    <t>tste_16_9</t>
+  </si>
+  <si>
+    <t>tste_16_10</t>
+  </si>
+  <si>
+    <t>tste_16_12</t>
+  </si>
+  <si>
+    <t>tste_16_13</t>
+  </si>
+  <si>
+    <t>tste_16_14</t>
+  </si>
+  <si>
+    <t>tste_16_15</t>
+  </si>
+  <si>
+    <t>tste_16_11</t>
+  </si>
+  <si>
+    <t>tste_16_0*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_16_1*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_16_2*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_16_3*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_16_4*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_16_5*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_16_6*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_16_7*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_16_8*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_16_9*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_16_10*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_16_11*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_16_12*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_16_13*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_16_14*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_16_15*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_16_0*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_16_1*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_16_2*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_16_3*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_16_4*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_16_5*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_16_6*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_16_7*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_16_8*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_16_9*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_16_10*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_16_11*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_16_12*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_16_13*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_16_14*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_16_15*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_16_0*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_16_1*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_16_2*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_16_3*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_16_4*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_16_5*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_16_6*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_16_7*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_16_8*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_16_9*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_16_10*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_16_11*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_16_12*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_16_13*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_16_14*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_16_15*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_16_0*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_16_1*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_16_2*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_16_3*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_16_4*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_16_5*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_16_6*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_16_7*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_16_8*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_16_9*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_16_10*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_16_11*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_16_12*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_16_13*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_16_14*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_16_15*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_16_0*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_16_1*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_16_2*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_16_3*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_16_4*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_16_5*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_16_6*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_16_7*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_16_8*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_16_9*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_16_10*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_16_11*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_16_12*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_16_13*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_16_14*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_16_15*gap_openness</t>
   </si>
 </sst>
 </file>
@@ -1789,10 +2410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V116"/>
+  <dimension ref="A1:AA116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X23" sqref="X23"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X9" sqref="X9:Y9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1807,10 +2428,11 @@
     <col min="16" max="16" width="28.453125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="28.453125" customWidth="1"/>
     <col min="18" max="21" width="28.453125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="28.453125" customWidth="1"/>
+    <col min="22" max="24" width="28.453125" customWidth="1"/>
+    <col min="25" max="27" width="26.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1859,8 +2481,23 @@
       <c r="V1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W1" t="s">
+        <v>12</v>
+      </c>
+      <c r="X1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1909,8 +2546,23 @@
       <c r="V2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W2" t="s">
+        <v>13</v>
+      </c>
+      <c r="X2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1959,8 +2611,23 @@
       <c r="V3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W3" t="s">
+        <v>14</v>
+      </c>
+      <c r="X3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2006,8 +2673,23 @@
       <c r="V4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W4" t="s">
+        <v>15</v>
+      </c>
+      <c r="X4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -2053,8 +2735,23 @@
       <c r="V5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W5" t="s">
+        <v>16</v>
+      </c>
+      <c r="X5" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -2103,8 +2800,23 @@
       <c r="V6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W6" t="s">
+        <v>17</v>
+      </c>
+      <c r="X6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -2153,8 +2865,23 @@
       <c r="V7" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W7" t="s">
+        <v>181</v>
+      </c>
+      <c r="X7" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>181</v>
       </c>
@@ -2203,8 +2930,23 @@
       <c r="V8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W8" t="s">
+        <v>7</v>
+      </c>
+      <c r="X8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2253,8 +2995,23 @@
       <c r="V9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W9" t="s">
+        <v>8</v>
+      </c>
+      <c r="X9" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2303,8 +3060,23 @@
       <c r="V10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W10" t="s">
+        <v>9</v>
+      </c>
+      <c r="X10" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2350,8 +3122,23 @@
       <c r="V11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W11" t="s">
+        <v>10</v>
+      </c>
+      <c r="X11" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2394,8 +3181,23 @@
       <c r="V12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W12" t="s">
+        <v>11</v>
+      </c>
+      <c r="X12" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2438,8 +3240,23 @@
       <c r="V13" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W13" t="s">
+        <v>59</v>
+      </c>
+      <c r="X13" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -2482,8 +3299,23 @@
       <c r="V14" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W14" t="s">
+        <v>60</v>
+      </c>
+      <c r="X14" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -2526,8 +3358,23 @@
       <c r="V15" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W15" t="s">
+        <v>61</v>
+      </c>
+      <c r="X15" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -2570,8 +3417,23 @@
       <c r="V16" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W16" t="s">
+        <v>62</v>
+      </c>
+      <c r="X16" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -2614,8 +3476,23 @@
       <c r="V17" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W17" t="s">
+        <v>63</v>
+      </c>
+      <c r="X17" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -2658,8 +3535,23 @@
       <c r="V18" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W18" t="s">
+        <v>288</v>
+      </c>
+      <c r="X18" t="s">
+        <v>288</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>527</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>527</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -2702,8 +3594,23 @@
       <c r="V19" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W19" t="s">
+        <v>289</v>
+      </c>
+      <c r="X19" t="s">
+        <v>289</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>528</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>528</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -2746,8 +3653,23 @@
       <c r="V20" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W20" t="s">
+        <v>290</v>
+      </c>
+      <c r="X20" t="s">
+        <v>290</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>529</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>529</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -2790,8 +3712,23 @@
       <c r="V21" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W21" t="s">
+        <v>291</v>
+      </c>
+      <c r="X21" t="s">
+        <v>291</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>530</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>530</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -2831,8 +3768,23 @@
       <c r="V22" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W22" t="s">
+        <v>292</v>
+      </c>
+      <c r="X22" t="s">
+        <v>292</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>531</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>531</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -2872,8 +3824,23 @@
       <c r="V23" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W23" t="s">
+        <v>293</v>
+      </c>
+      <c r="X23" t="s">
+        <v>293</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>532</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>532</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -2913,8 +3880,23 @@
       <c r="V24" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W24" t="s">
+        <v>294</v>
+      </c>
+      <c r="X24" t="s">
+        <v>294</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>533</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>533</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>65</v>
       </c>
@@ -2954,8 +3936,23 @@
       <c r="V25" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W25" t="s">
+        <v>295</v>
+      </c>
+      <c r="X25" t="s">
+        <v>295</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>534</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>534</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -2995,8 +3992,23 @@
       <c r="V26" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W26" t="s">
+        <v>296</v>
+      </c>
+      <c r="X26" t="s">
+        <v>296</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>535</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>535</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -3036,8 +4048,23 @@
       <c r="V27" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W27" t="s">
+        <v>482</v>
+      </c>
+      <c r="X27" t="s">
+        <v>482</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>536</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>536</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>68</v>
       </c>
@@ -3074,8 +4101,23 @@
       <c r="V28" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W28" t="s">
+        <v>483</v>
+      </c>
+      <c r="X28" t="s">
+        <v>483</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>537</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>537</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -3112,8 +4154,23 @@
       <c r="V29" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W29" t="s">
+        <v>484</v>
+      </c>
+      <c r="X29" t="s">
+        <v>484</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>538</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>538</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>70</v>
       </c>
@@ -3147,8 +4204,23 @@
       <c r="V30" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W30" t="s">
+        <v>485</v>
+      </c>
+      <c r="X30" t="s">
+        <v>485</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>539</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>539</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>71</v>
       </c>
@@ -3182,8 +4254,23 @@
       <c r="V31" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W31" t="s">
+        <v>486</v>
+      </c>
+      <c r="X31" t="s">
+        <v>486</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>540</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>540</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>72</v>
       </c>
@@ -3217,8 +4304,23 @@
       <c r="V32" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W32" t="s">
+        <v>487</v>
+      </c>
+      <c r="X32" t="s">
+        <v>487</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>541</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>541</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -3252,8 +4354,23 @@
       <c r="V33" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W33" t="s">
+        <v>488</v>
+      </c>
+      <c r="X33" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>542</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>542</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -3287,8 +4404,23 @@
       <c r="V34" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W34" t="s">
+        <v>489</v>
+      </c>
+      <c r="X34" t="s">
+        <v>489</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>543</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>543</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -3322,8 +4454,23 @@
       <c r="V35" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W35" t="s">
+        <v>522</v>
+      </c>
+      <c r="X35" t="s">
+        <v>522</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>544</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>544</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>3</v>
       </c>
@@ -3351,8 +4498,23 @@
       <c r="V36" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W36" t="s">
+        <v>490</v>
+      </c>
+      <c r="X36" t="s">
+        <v>490</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>545</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>545</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -3380,8 +4542,23 @@
       <c r="V37" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W37" t="s">
+        <v>491</v>
+      </c>
+      <c r="X37" t="s">
+        <v>491</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>546</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>546</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -3409,8 +4586,23 @@
       <c r="V38" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W38" t="s">
+        <v>492</v>
+      </c>
+      <c r="X38" t="s">
+        <v>492</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>547</v>
+      </c>
+      <c r="Z38" t="s">
+        <v>547</v>
+      </c>
+      <c r="AA38" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -3438,8 +4630,23 @@
       <c r="V39" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W39" t="s">
+        <v>493</v>
+      </c>
+      <c r="X39" t="s">
+        <v>493</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>548</v>
+      </c>
+      <c r="Z39" t="s">
+        <v>548</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>75</v>
       </c>
@@ -3467,8 +4674,23 @@
       <c r="V40" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W40" t="s">
+        <v>494</v>
+      </c>
+      <c r="X40" t="s">
+        <v>494</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>549</v>
+      </c>
+      <c r="Z40" t="s">
+        <v>549</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>76</v>
       </c>
@@ -3496,8 +4718,23 @@
       <c r="V41" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W41" t="s">
+        <v>495</v>
+      </c>
+      <c r="X41" t="s">
+        <v>495</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>550</v>
+      </c>
+      <c r="Z41" t="s">
+        <v>550</v>
+      </c>
+      <c r="AA41" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>77</v>
       </c>
@@ -3522,8 +4759,23 @@
       <c r="V42" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W42" t="s">
+        <v>496</v>
+      </c>
+      <c r="X42" t="s">
+        <v>496</v>
+      </c>
+      <c r="Y42" t="s">
+        <v>551</v>
+      </c>
+      <c r="Z42" t="s">
+        <v>551</v>
+      </c>
+      <c r="AA42" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>78</v>
       </c>
@@ -3548,8 +4800,23 @@
       <c r="V43" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W43" t="s">
+        <v>497</v>
+      </c>
+      <c r="X43" t="s">
+        <v>497</v>
+      </c>
+      <c r="Y43" t="s">
+        <v>552</v>
+      </c>
+      <c r="Z43" t="s">
+        <v>552</v>
+      </c>
+      <c r="AA43" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>79</v>
       </c>
@@ -3574,8 +4841,23 @@
       <c r="V44" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W44" t="s">
+        <v>523</v>
+      </c>
+      <c r="X44" t="s">
+        <v>523</v>
+      </c>
+      <c r="Y44" t="s">
+        <v>553</v>
+      </c>
+      <c r="Z44" t="s">
+        <v>553</v>
+      </c>
+      <c r="AA44" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>80</v>
       </c>
@@ -3600,8 +4882,23 @@
       <c r="V45" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W45" t="s">
+        <v>498</v>
+      </c>
+      <c r="X45" t="s">
+        <v>498</v>
+      </c>
+      <c r="Y45" t="s">
+        <v>554</v>
+      </c>
+      <c r="Z45" t="s">
+        <v>554</v>
+      </c>
+      <c r="AA45" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>81</v>
       </c>
@@ -3626,8 +4923,23 @@
       <c r="V46" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W46" t="s">
+        <v>499</v>
+      </c>
+      <c r="X46" t="s">
+        <v>499</v>
+      </c>
+      <c r="Y46" t="s">
+        <v>555</v>
+      </c>
+      <c r="Z46" t="s">
+        <v>555</v>
+      </c>
+      <c r="AA46" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>82</v>
       </c>
@@ -3652,8 +4964,23 @@
       <c r="V47" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W47" t="s">
+        <v>500</v>
+      </c>
+      <c r="X47" t="s">
+        <v>500</v>
+      </c>
+      <c r="Y47" t="s">
+        <v>556</v>
+      </c>
+      <c r="Z47" t="s">
+        <v>556</v>
+      </c>
+      <c r="AA47" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>83</v>
       </c>
@@ -3675,8 +5002,23 @@
       <c r="V48" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W48" t="s">
+        <v>501</v>
+      </c>
+      <c r="X48" t="s">
+        <v>501</v>
+      </c>
+      <c r="Y48" t="s">
+        <v>557</v>
+      </c>
+      <c r="Z48" t="s">
+        <v>557</v>
+      </c>
+      <c r="AA48" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>84</v>
       </c>
@@ -3698,8 +5040,23 @@
       <c r="V49" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W49" t="s">
+        <v>502</v>
+      </c>
+      <c r="X49" t="s">
+        <v>502</v>
+      </c>
+      <c r="Y49" t="s">
+        <v>558</v>
+      </c>
+      <c r="Z49" t="s">
+        <v>558</v>
+      </c>
+      <c r="AA49" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>85</v>
       </c>
@@ -3721,8 +5078,23 @@
       <c r="V50" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W50" t="s">
+        <v>503</v>
+      </c>
+      <c r="X50" t="s">
+        <v>503</v>
+      </c>
+      <c r="Y50" t="s">
+        <v>559</v>
+      </c>
+      <c r="Z50" t="s">
+        <v>559</v>
+      </c>
+      <c r="AA50" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>86</v>
       </c>
@@ -3744,8 +5116,23 @@
       <c r="V51" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W51" t="s">
+        <v>504</v>
+      </c>
+      <c r="X51" t="s">
+        <v>504</v>
+      </c>
+      <c r="Y51" t="s">
+        <v>560</v>
+      </c>
+      <c r="Z51" t="s">
+        <v>560</v>
+      </c>
+      <c r="AA51" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="52" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>87</v>
       </c>
@@ -3764,8 +5151,23 @@
       <c r="V52" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W52" t="s">
+        <v>505</v>
+      </c>
+      <c r="X52" t="s">
+        <v>505</v>
+      </c>
+      <c r="Y52" t="s">
+        <v>561</v>
+      </c>
+      <c r="Z52" t="s">
+        <v>561</v>
+      </c>
+      <c r="AA52" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="53" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>88</v>
       </c>
@@ -3784,8 +5186,23 @@
       <c r="V53" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W53" t="s">
+        <v>524</v>
+      </c>
+      <c r="X53" t="s">
+        <v>524</v>
+      </c>
+      <c r="Y53" t="s">
+        <v>562</v>
+      </c>
+      <c r="Z53" t="s">
+        <v>562</v>
+      </c>
+      <c r="AA53" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="54" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>89</v>
       </c>
@@ -3801,8 +5218,23 @@
       <c r="V54" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W54" t="s">
+        <v>506</v>
+      </c>
+      <c r="X54" t="s">
+        <v>506</v>
+      </c>
+      <c r="Y54" t="s">
+        <v>563</v>
+      </c>
+      <c r="Z54" t="s">
+        <v>563</v>
+      </c>
+      <c r="AA54" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="55" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>90</v>
       </c>
@@ -3818,8 +5250,23 @@
       <c r="V55" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W55" t="s">
+        <v>507</v>
+      </c>
+      <c r="X55" t="s">
+        <v>507</v>
+      </c>
+      <c r="Y55" t="s">
+        <v>564</v>
+      </c>
+      <c r="Z55" t="s">
+        <v>564</v>
+      </c>
+      <c r="AA55" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="56" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>91</v>
       </c>
@@ -3835,8 +5282,23 @@
       <c r="V56" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W56" t="s">
+        <v>508</v>
+      </c>
+      <c r="X56" t="s">
+        <v>508</v>
+      </c>
+      <c r="Y56" t="s">
+        <v>565</v>
+      </c>
+      <c r="Z56" t="s">
+        <v>565</v>
+      </c>
+      <c r="AA56" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="57" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>92</v>
       </c>
@@ -3852,8 +5314,23 @@
       <c r="V57" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W57" t="s">
+        <v>509</v>
+      </c>
+      <c r="X57" t="s">
+        <v>509</v>
+      </c>
+      <c r="Y57" t="s">
+        <v>566</v>
+      </c>
+      <c r="Z57" t="s">
+        <v>566</v>
+      </c>
+      <c r="AA57" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="58" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>93</v>
       </c>
@@ -3869,8 +5346,23 @@
       <c r="V58" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W58" t="s">
+        <v>510</v>
+      </c>
+      <c r="X58" t="s">
+        <v>510</v>
+      </c>
+      <c r="Y58" t="s">
+        <v>567</v>
+      </c>
+      <c r="Z58" t="s">
+        <v>567</v>
+      </c>
+      <c r="AA58" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="59" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>94</v>
       </c>
@@ -3886,8 +5378,23 @@
       <c r="V59" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W59" t="s">
+        <v>511</v>
+      </c>
+      <c r="X59" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y59" t="s">
+        <v>568</v>
+      </c>
+      <c r="Z59" t="s">
+        <v>568</v>
+      </c>
+      <c r="AA59" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="60" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>95</v>
       </c>
@@ -3900,8 +5407,23 @@
       <c r="V60" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W60" t="s">
+        <v>512</v>
+      </c>
+      <c r="X60" t="s">
+        <v>512</v>
+      </c>
+      <c r="Y60" t="s">
+        <v>569</v>
+      </c>
+      <c r="Z60" t="s">
+        <v>569</v>
+      </c>
+      <c r="AA60" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="61" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>73</v>
       </c>
@@ -3914,8 +5436,23 @@
       <c r="V61" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W61" t="s">
+        <v>513</v>
+      </c>
+      <c r="X61" t="s">
+        <v>513</v>
+      </c>
+      <c r="Y61" t="s">
+        <v>570</v>
+      </c>
+      <c r="Z61" t="s">
+        <v>570</v>
+      </c>
+      <c r="AA61" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="62" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>74</v>
       </c>
@@ -3928,8 +5465,23 @@
       <c r="V62" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W62" t="s">
+        <v>525</v>
+      </c>
+      <c r="X62" t="s">
+        <v>525</v>
+      </c>
+      <c r="Y62" t="s">
+        <v>571</v>
+      </c>
+      <c r="Z62" t="s">
+        <v>571</v>
+      </c>
+      <c r="AA62" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="63" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>253</v>
       </c>
@@ -3942,8 +5494,23 @@
       <c r="V63" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W63" t="s">
+        <v>514</v>
+      </c>
+      <c r="X63" t="s">
+        <v>514</v>
+      </c>
+      <c r="Y63" t="s">
+        <v>572</v>
+      </c>
+      <c r="Z63" t="s">
+        <v>572</v>
+      </c>
+      <c r="AA63" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="64" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>254</v>
       </c>
@@ -3956,8 +5523,23 @@
       <c r="V64" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W64" t="s">
+        <v>515</v>
+      </c>
+      <c r="X64" t="s">
+        <v>515</v>
+      </c>
+      <c r="Y64" t="s">
+        <v>573</v>
+      </c>
+      <c r="Z64" t="s">
+        <v>573</v>
+      </c>
+      <c r="AA64" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="65" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>255</v>
       </c>
@@ -3970,8 +5552,23 @@
       <c r="V65" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W65" t="s">
+        <v>516</v>
+      </c>
+      <c r="X65" t="s">
+        <v>516</v>
+      </c>
+      <c r="Y65" t="s">
+        <v>574</v>
+      </c>
+      <c r="Z65" t="s">
+        <v>574</v>
+      </c>
+      <c r="AA65" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="66" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>256</v>
       </c>
@@ -3981,8 +5578,23 @@
       <c r="N66" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W66" t="s">
+        <v>517</v>
+      </c>
+      <c r="X66" t="s">
+        <v>517</v>
+      </c>
+      <c r="Y66" t="s">
+        <v>575</v>
+      </c>
+      <c r="Z66" t="s">
+        <v>575</v>
+      </c>
+      <c r="AA66" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="67" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>257</v>
       </c>
@@ -3992,8 +5604,23 @@
       <c r="N67" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W67" t="s">
+        <v>518</v>
+      </c>
+      <c r="X67" t="s">
+        <v>518</v>
+      </c>
+      <c r="Y67" t="s">
+        <v>576</v>
+      </c>
+      <c r="Z67" t="s">
+        <v>576</v>
+      </c>
+      <c r="AA67" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="68" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>258</v>
       </c>
@@ -4003,8 +5630,23 @@
       <c r="N68" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W68" t="s">
+        <v>519</v>
+      </c>
+      <c r="X68" t="s">
+        <v>519</v>
+      </c>
+      <c r="Y68" t="s">
+        <v>577</v>
+      </c>
+      <c r="Z68" t="s">
+        <v>577</v>
+      </c>
+      <c r="AA68" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="69" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>259</v>
       </c>
@@ -4014,8 +5656,23 @@
       <c r="N69" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W69" t="s">
+        <v>520</v>
+      </c>
+      <c r="X69" t="s">
+        <v>520</v>
+      </c>
+      <c r="Y69" t="s">
+        <v>578</v>
+      </c>
+      <c r="Z69" t="s">
+        <v>578</v>
+      </c>
+      <c r="AA69" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="70" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>260</v>
       </c>
@@ -4025,8 +5682,23 @@
       <c r="N70" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W70" t="s">
+        <v>521</v>
+      </c>
+      <c r="X70" t="s">
+        <v>521</v>
+      </c>
+      <c r="Y70" t="s">
+        <v>579</v>
+      </c>
+      <c r="Z70" t="s">
+        <v>579</v>
+      </c>
+      <c r="AA70" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="71" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>261</v>
       </c>
@@ -4036,8 +5708,23 @@
       <c r="N71" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W71" t="s">
+        <v>526</v>
+      </c>
+      <c r="X71" t="s">
+        <v>526</v>
+      </c>
+      <c r="Y71" t="s">
+        <v>580</v>
+      </c>
+      <c r="Z71" t="s">
+        <v>580</v>
+      </c>
+      <c r="AA71" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="72" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>262</v>
       </c>
@@ -4047,8 +5734,17 @@
       <c r="N72" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="Y72" t="s">
+        <v>581</v>
+      </c>
+      <c r="Z72" t="s">
+        <v>581</v>
+      </c>
+      <c r="AA72" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="73" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>263</v>
       </c>
@@ -4058,8 +5754,17 @@
       <c r="N73" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="Y73" t="s">
+        <v>582</v>
+      </c>
+      <c r="Z73" t="s">
+        <v>582</v>
+      </c>
+      <c r="AA73" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="74" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>264</v>
       </c>
@@ -4069,8 +5774,17 @@
       <c r="N74" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="Y74" t="s">
+        <v>583</v>
+      </c>
+      <c r="Z74" t="s">
+        <v>583</v>
+      </c>
+      <c r="AA74" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="75" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>265</v>
       </c>
@@ -4080,211 +5794,382 @@
       <c r="N75" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="Y75" t="s">
+        <v>584</v>
+      </c>
+      <c r="Z75" t="s">
+        <v>584</v>
+      </c>
+      <c r="AA75" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="76" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>266</v>
       </c>
       <c r="N76" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="Y76" t="s">
+        <v>585</v>
+      </c>
+      <c r="Z76" t="s">
+        <v>585</v>
+      </c>
+      <c r="AA76" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="77" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="Y77" t="s">
+        <v>586</v>
+      </c>
+      <c r="Z77" t="s">
+        <v>586</v>
+      </c>
+      <c r="AA77" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="78" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="Y78" t="s">
+        <v>587</v>
+      </c>
+      <c r="Z78" t="s">
+        <v>587</v>
+      </c>
+      <c r="AA78" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="79" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="Y79" t="s">
+        <v>588</v>
+      </c>
+      <c r="Z79" t="s">
+        <v>588</v>
+      </c>
+      <c r="AA79" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="80" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="Y80" t="s">
+        <v>589</v>
+      </c>
+      <c r="Z80" t="s">
+        <v>589</v>
+      </c>
+      <c r="AA80" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="81" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="Y81" t="s">
+        <v>590</v>
+      </c>
+      <c r="Z81" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA81" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="82" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="Y82" t="s">
+        <v>591</v>
+      </c>
+      <c r="Z82" t="s">
+        <v>591</v>
+      </c>
+      <c r="AA82" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="83" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="Y83" t="s">
+        <v>592</v>
+      </c>
+      <c r="Z83" t="s">
+        <v>592</v>
+      </c>
+      <c r="AA83" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="84" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA84" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="85" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA85" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="86" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA86" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="87" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA87" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="88" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA88" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="89" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA89" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="90" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA90" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="91" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA91" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="92" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA92" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="93" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA93" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="94" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA94" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="95" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA95" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="96" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA96" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="97" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA97" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="98" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA98" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="99" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA99" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="100" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA100" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="101" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA101" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="102" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA102" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="103" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA103" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="104" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA104" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="105" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA105" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="106" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA106" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="107" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA107" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="108" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA108" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="109" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA109" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="110" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA110" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="111" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA111" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="112" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA112" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="113" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="AA113" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="114" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>306</v>
       </c>

</xml_diff>

<commit_message>
Add persoality dis; complete the BIC and AIC from model 2-20
</commit_message>
<xml_diff>
--- a/data/vars/combination.xlsx
+++ b/data/vars/combination.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="10170" yWindow="0" windowWidth="22260" windowHeight="12653"/>
+    <workbookView xWindow="12130" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="949">
   <si>
     <t>distance_survey_mean_1</t>
   </si>
@@ -2236,6 +2236,636 @@
   </si>
   <si>
     <t>tste_10_9*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_17_0</t>
+  </si>
+  <si>
+    <t>tste_17_1</t>
+  </si>
+  <si>
+    <t>tste_17_2</t>
+  </si>
+  <si>
+    <t>tste_17_3</t>
+  </si>
+  <si>
+    <t>tste_17_4</t>
+  </si>
+  <si>
+    <t>tste_17_5</t>
+  </si>
+  <si>
+    <t>tste_17_6</t>
+  </si>
+  <si>
+    <t>tste_17_7</t>
+  </si>
+  <si>
+    <t>tste_17_8</t>
+  </si>
+  <si>
+    <t>tste_17_9</t>
+  </si>
+  <si>
+    <t>tste_17_10</t>
+  </si>
+  <si>
+    <t>tste_17_11</t>
+  </si>
+  <si>
+    <t>tste_17_12</t>
+  </si>
+  <si>
+    <t>tste_17_13</t>
+  </si>
+  <si>
+    <t>tste_17_14</t>
+  </si>
+  <si>
+    <t>tste_17_15</t>
+  </si>
+  <si>
+    <t>tste_17_16</t>
+  </si>
+  <si>
+    <t>tste_17_0*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_17_1*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_17_2*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_17_3*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_17_4*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_17_5*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_17_6*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_17_7*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_17_8*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_17_9*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_17_10*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_17_11*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_17_12*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_17_13*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_17_14*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_17_15*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_17_16*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_17_0*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_17_1*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_17_2*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_17_3*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_17_4*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_17_5*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_17_6*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_17_7*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_17_8*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_17_9*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_17_10*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_17_11*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_17_12*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_17_13*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_17_14*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_17_15*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_17_16*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_17_0*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_17_1*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_17_2*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_17_3*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_17_4*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_17_5*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_17_6*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_17_7*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_17_8*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_17_9*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_17_10*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_17_11*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_17_12*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_17_13*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_17_14*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_17_15*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_17_16*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_17_0*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_17_1*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_17_2*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_17_3*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_17_4*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_17_5*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_17_6*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_17_7*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_17_8*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_17_9*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_17_10*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_17_11*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_17_12*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_17_13*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_17_14*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_17_15*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_17_16*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_17_0*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_17_1*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_17_2*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_17_3*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_17_4*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_17_5*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_17_6*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_17_7*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_17_8*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_17_9*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_17_10*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_17_11*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_17_12*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_17_13*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_17_14*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_17_15*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_17_16*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_18_0</t>
+  </si>
+  <si>
+    <t>tste_18_1</t>
+  </si>
+  <si>
+    <t>tste_18_2</t>
+  </si>
+  <si>
+    <t>tste_18_3</t>
+  </si>
+  <si>
+    <t>tste_18_4</t>
+  </si>
+  <si>
+    <t>tste_18_5</t>
+  </si>
+  <si>
+    <t>tste_18_6</t>
+  </si>
+  <si>
+    <t>tste_18_7</t>
+  </si>
+  <si>
+    <t>tste_18_8</t>
+  </si>
+  <si>
+    <t>tste_18_9</t>
+  </si>
+  <si>
+    <t>tste_18_10</t>
+  </si>
+  <si>
+    <t>tste_18_11</t>
+  </si>
+  <si>
+    <t>tste_18_12</t>
+  </si>
+  <si>
+    <t>tste_18_13</t>
+  </si>
+  <si>
+    <t>tste_18_14</t>
+  </si>
+  <si>
+    <t>tste_18_15</t>
+  </si>
+  <si>
+    <t>tste_18_16</t>
+  </si>
+  <si>
+    <t>tste_18_17</t>
+  </si>
+  <si>
+    <t>tste_18_0*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_18_1*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_18_2*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_18_3*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_18_4*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_18_5*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_18_6*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_18_7*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_18_8*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_18_9*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_18_10*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_18_11*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_18_12*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_18_13*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_18_14*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_18_15*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_18_16*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_18_17*gap_extraversion</t>
+  </si>
+  <si>
+    <t>tste_18_0*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_18_1*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_18_2*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_18_3*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_18_4*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_18_5*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_18_6*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_18_7*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_18_8*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_18_9*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_18_10*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_18_11*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_18_12*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_18_13*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_18_14*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_18_15*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_18_16*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_18_17*gap_agreeableness</t>
+  </si>
+  <si>
+    <t>tste_18_0*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_18_1*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_18_2*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_18_3*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_18_4*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_18_5*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_18_6*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_18_7*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_18_8*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_18_9*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_18_10*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_18_11*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_18_12*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_18_13*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_18_14*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_18_15*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_18_16*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_18_17*gap_conscientiousness</t>
+  </si>
+  <si>
+    <t>tste_18_0*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_18_1*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_18_2*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_18_3*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_18_4*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_18_5*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_18_6*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_18_7*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_18_8*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_18_9*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_18_10*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_18_11*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_18_12*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_18_13*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_18_14*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_18_15*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_18_16*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_18_17*gap_emotionstability</t>
+  </si>
+  <si>
+    <t>tste_18_0*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_18_1*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_18_2*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_18_3*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_18_4*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_18_5*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_18_6*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_18_7*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_18_8*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_18_9*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_18_10*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_18_11*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_18_12*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_18_13*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_18_14*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_18_15*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_18_16*gap_openness</t>
+  </si>
+  <si>
+    <t>tste_18_17*gap_openness</t>
   </si>
 </sst>
 </file>
@@ -2560,29 +3190,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z116"/>
+  <dimension ref="A1:AB125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC18" sqref="AC18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="5" max="5" width="43" customWidth="1"/>
-    <col min="7" max="7" width="42.06640625" customWidth="1"/>
-    <col min="9" max="9" width="34.73046875" customWidth="1"/>
-    <col min="10" max="10" width="1.73046875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="32.796875" customWidth="1"/>
-    <col min="12" max="12" width="45.19921875" customWidth="1"/>
-    <col min="13" max="15" width="45.06640625" customWidth="1"/>
-    <col min="16" max="16" width="28.46484375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.46484375" customWidth="1"/>
-    <col min="18" max="21" width="28.46484375" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="28.46484375" customWidth="1"/>
-    <col min="24" max="26" width="26.19921875" customWidth="1"/>
+    <col min="7" max="7" width="42.08984375" customWidth="1"/>
+    <col min="9" max="9" width="34.7265625" customWidth="1"/>
+    <col min="10" max="10" width="1.7265625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="32.81640625" customWidth="1"/>
+    <col min="12" max="12" width="45.1796875" customWidth="1"/>
+    <col min="13" max="15" width="45.08984375" customWidth="1"/>
+    <col min="16" max="16" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.453125" customWidth="1"/>
+    <col min="18" max="21" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="28.453125" customWidth="1"/>
+    <col min="24" max="28" width="26.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -2643,8 +3273,14 @@
       <c r="Z1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -2705,8 +3341,14 @@
       <c r="Z2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2767,8 +3409,14 @@
       <c r="Z3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2826,8 +3474,14 @@
       <c r="Z4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -2885,8 +3539,14 @@
       <c r="Z5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -2947,8 +3607,14 @@
       <c r="Z6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -3009,8 +3675,14 @@
       <c r="Z7" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA7" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>181</v>
       </c>
@@ -3071,8 +3743,14 @@
       <c r="Z8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA8" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -3133,8 +3811,14 @@
       <c r="Z9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA9" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3195,8 +3879,14 @@
       <c r="Z10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA10" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -3254,8 +3944,14 @@
       <c r="Z11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA11" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -3310,8 +4006,14 @@
       <c r="Z12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA12" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -3366,8 +4068,14 @@
       <c r="Z13" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA13" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -3422,8 +4130,14 @@
       <c r="Z14" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA14" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -3478,8 +4192,14 @@
       <c r="Z15" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA15" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -3534,8 +4254,14 @@
       <c r="Z16" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA16" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -3590,8 +4316,14 @@
       <c r="Z17" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA17" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -3646,8 +4378,14 @@
       <c r="Z18" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA18" t="s">
+        <v>739</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -3702,8 +4440,14 @@
       <c r="Z19" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA19" t="s">
+        <v>740</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -3758,8 +4502,14 @@
       <c r="Z20" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA20" t="s">
+        <v>741</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -3814,8 +4564,14 @@
       <c r="Z21" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA21" t="s">
+        <v>742</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -3867,8 +4623,14 @@
       <c r="Z22" t="s">
         <v>597</v>
       </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA22" t="s">
+        <v>743</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -3920,8 +4682,14 @@
       <c r="Z23" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA23" t="s">
+        <v>744</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -3973,8 +4741,14 @@
       <c r="Z24" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA24" t="s">
+        <v>745</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>65</v>
       </c>
@@ -4026,8 +4800,14 @@
       <c r="Z25" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA25" t="s">
+        <v>746</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -4079,8 +4859,14 @@
       <c r="Z26" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA26" t="s">
+        <v>747</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -4132,8 +4918,14 @@
       <c r="Z27" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA27" t="s">
+        <v>748</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>68</v>
       </c>
@@ -4182,8 +4974,14 @@
       <c r="Z28" t="s">
         <v>603</v>
       </c>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA28" t="s">
+        <v>749</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -4232,8 +5030,14 @@
       <c r="Z29" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA29" t="s">
+        <v>750</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>70</v>
       </c>
@@ -4279,8 +5083,14 @@
       <c r="Z30" t="s">
         <v>604</v>
       </c>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA30" t="s">
+        <v>751</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>71</v>
       </c>
@@ -4326,8 +5136,14 @@
       <c r="Z31" t="s">
         <v>605</v>
       </c>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA31" t="s">
+        <v>752</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>72</v>
       </c>
@@ -4373,8 +5189,14 @@
       <c r="Z32" t="s">
         <v>606</v>
       </c>
-    </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA32" t="s">
+        <v>753</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -4420,8 +5242,14 @@
       <c r="Z33" t="s">
         <v>607</v>
       </c>
-    </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA33" t="s">
+        <v>754</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -4467,8 +5295,14 @@
       <c r="Z34" t="s">
         <v>609</v>
       </c>
-    </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA34" t="s">
+        <v>755</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -4514,8 +5348,14 @@
       <c r="Z35" t="s">
         <v>610</v>
       </c>
-    </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA35" t="s">
+        <v>756</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>3</v>
       </c>
@@ -4555,8 +5395,14 @@
       <c r="Z36" t="s">
         <v>611</v>
       </c>
-    </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA36" t="s">
+        <v>757</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -4596,8 +5442,14 @@
       <c r="Z37" t="s">
         <v>612</v>
       </c>
-    </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA37" t="s">
+        <v>758</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -4637,8 +5489,14 @@
       <c r="Z38" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA38" t="s">
+        <v>759</v>
+      </c>
+      <c r="AB38" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -4678,8 +5536,14 @@
       <c r="Z39" t="s">
         <v>614</v>
       </c>
-    </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA39" t="s">
+        <v>760</v>
+      </c>
+      <c r="AB39" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>75</v>
       </c>
@@ -4719,8 +5583,14 @@
       <c r="Z40" t="s">
         <v>615</v>
       </c>
-    </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA40" t="s">
+        <v>761</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>76</v>
       </c>
@@ -4760,8 +5630,14 @@
       <c r="Z41" t="s">
         <v>616</v>
       </c>
-    </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA41" t="s">
+        <v>762</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>77</v>
       </c>
@@ -4798,8 +5674,14 @@
       <c r="Z42" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA42" t="s">
+        <v>763</v>
+      </c>
+      <c r="AB42" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>78</v>
       </c>
@@ -4836,8 +5718,14 @@
       <c r="Z43" t="s">
         <v>618</v>
       </c>
-    </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA43" t="s">
+        <v>764</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>79</v>
       </c>
@@ -4874,8 +5762,14 @@
       <c r="Z44" t="s">
         <v>619</v>
       </c>
-    </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA44" t="s">
+        <v>765</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>80</v>
       </c>
@@ -4912,8 +5806,14 @@
       <c r="Z45" t="s">
         <v>620</v>
       </c>
-    </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA45" t="s">
+        <v>766</v>
+      </c>
+      <c r="AB45" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>81</v>
       </c>
@@ -4950,8 +5850,14 @@
       <c r="Z46" t="s">
         <v>621</v>
       </c>
-    </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA46" t="s">
+        <v>767</v>
+      </c>
+      <c r="AB46" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>82</v>
       </c>
@@ -4988,8 +5894,14 @@
       <c r="Z47" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA47" t="s">
+        <v>768</v>
+      </c>
+      <c r="AB47" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>83</v>
       </c>
@@ -5023,8 +5935,14 @@
       <c r="Z48" t="s">
         <v>623</v>
       </c>
-    </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA48" t="s">
+        <v>769</v>
+      </c>
+      <c r="AB48" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>84</v>
       </c>
@@ -5058,8 +5976,14 @@
       <c r="Z49" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA49" t="s">
+        <v>770</v>
+      </c>
+      <c r="AB49" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>85</v>
       </c>
@@ -5093,8 +6017,14 @@
       <c r="Z50" t="s">
         <v>625</v>
       </c>
-    </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA50" t="s">
+        <v>771</v>
+      </c>
+      <c r="AB50" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>86</v>
       </c>
@@ -5128,8 +6058,14 @@
       <c r="Z51" t="s">
         <v>626</v>
       </c>
-    </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA51" t="s">
+        <v>772</v>
+      </c>
+      <c r="AB51" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>87</v>
       </c>
@@ -5160,8 +6096,14 @@
       <c r="Z52" t="s">
         <v>627</v>
       </c>
-    </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA52" t="s">
+        <v>773</v>
+      </c>
+      <c r="AB52" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="53" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>88</v>
       </c>
@@ -5192,8 +6134,14 @@
       <c r="Z53" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA53" t="s">
+        <v>774</v>
+      </c>
+      <c r="AB53" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="54" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>89</v>
       </c>
@@ -5221,8 +6169,14 @@
       <c r="Z54" t="s">
         <v>629</v>
       </c>
-    </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA54" t="s">
+        <v>775</v>
+      </c>
+      <c r="AB54" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="55" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>90</v>
       </c>
@@ -5250,8 +6204,14 @@
       <c r="Z55" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA55" t="s">
+        <v>776</v>
+      </c>
+      <c r="AB55" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="56" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>91</v>
       </c>
@@ -5279,8 +6239,14 @@
       <c r="Z56" t="s">
         <v>631</v>
       </c>
-    </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA56" t="s">
+        <v>777</v>
+      </c>
+      <c r="AB56" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="57" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>92</v>
       </c>
@@ -5308,8 +6274,14 @@
       <c r="Z57" t="s">
         <v>632</v>
       </c>
-    </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA57" t="s">
+        <v>778</v>
+      </c>
+      <c r="AB57" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="58" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>93</v>
       </c>
@@ -5337,8 +6309,14 @@
       <c r="Z58" t="s">
         <v>633</v>
       </c>
-    </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA58" t="s">
+        <v>779</v>
+      </c>
+      <c r="AB58" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="59" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>94</v>
       </c>
@@ -5366,8 +6344,14 @@
       <c r="Z59" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA59" t="s">
+        <v>780</v>
+      </c>
+      <c r="AB59" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="60" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>95</v>
       </c>
@@ -5392,8 +6376,14 @@
       <c r="Z60" t="s">
         <v>635</v>
       </c>
-    </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA60" t="s">
+        <v>781</v>
+      </c>
+      <c r="AB60" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="61" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>73</v>
       </c>
@@ -5418,8 +6408,14 @@
       <c r="Z61" t="s">
         <v>636</v>
       </c>
-    </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA61" t="s">
+        <v>782</v>
+      </c>
+      <c r="AB61" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="62" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>74</v>
       </c>
@@ -5444,8 +6440,14 @@
       <c r="Z62" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA62" t="s">
+        <v>783</v>
+      </c>
+      <c r="AB62" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="63" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>253</v>
       </c>
@@ -5470,8 +6472,14 @@
       <c r="Z63" t="s">
         <v>638</v>
       </c>
-    </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA63" t="s">
+        <v>784</v>
+      </c>
+      <c r="AB63" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="64" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>254</v>
       </c>
@@ -5496,8 +6504,14 @@
       <c r="Z64" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA64" t="s">
+        <v>785</v>
+      </c>
+      <c r="AB64" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="65" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>255</v>
       </c>
@@ -5522,8 +6536,14 @@
       <c r="Z65" t="s">
         <v>640</v>
       </c>
-    </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA65" t="s">
+        <v>786</v>
+      </c>
+      <c r="AB65" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="66" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>256</v>
       </c>
@@ -5545,8 +6565,14 @@
       <c r="Z66" t="s">
         <v>641</v>
       </c>
-    </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA66" t="s">
+        <v>787</v>
+      </c>
+      <c r="AB66" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="67" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>257</v>
       </c>
@@ -5568,8 +6594,14 @@
       <c r="Z67" t="s">
         <v>642</v>
       </c>
-    </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA67" t="s">
+        <v>788</v>
+      </c>
+      <c r="AB67" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="68" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>258</v>
       </c>
@@ -5591,8 +6623,14 @@
       <c r="Z68" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA68" t="s">
+        <v>789</v>
+      </c>
+      <c r="AB68" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="69" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>259</v>
       </c>
@@ -5614,8 +6652,14 @@
       <c r="Z69" t="s">
         <v>644</v>
       </c>
-    </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA69" t="s">
+        <v>790</v>
+      </c>
+      <c r="AB69" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="70" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>260</v>
       </c>
@@ -5637,8 +6681,14 @@
       <c r="Z70" t="s">
         <v>645</v>
       </c>
-    </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA70" t="s">
+        <v>791</v>
+      </c>
+      <c r="AB70" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="71" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>261</v>
       </c>
@@ -5660,8 +6710,14 @@
       <c r="Z71" t="s">
         <v>646</v>
       </c>
-    </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA71" t="s">
+        <v>792</v>
+      </c>
+      <c r="AB71" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="72" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>262</v>
       </c>
@@ -5680,8 +6736,14 @@
       <c r="Z72" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA72" t="s">
+        <v>793</v>
+      </c>
+      <c r="AB72" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="73" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>263</v>
       </c>
@@ -5700,8 +6762,14 @@
       <c r="Z73" t="s">
         <v>648</v>
       </c>
-    </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA73" t="s">
+        <v>794</v>
+      </c>
+      <c r="AB73" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="74" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>264</v>
       </c>
@@ -5720,8 +6788,14 @@
       <c r="Z74" t="s">
         <v>649</v>
       </c>
-    </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA74" t="s">
+        <v>795</v>
+      </c>
+      <c r="AB74" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="75" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>265</v>
       </c>
@@ -5740,8 +6814,14 @@
       <c r="Z75" t="s">
         <v>650</v>
       </c>
-    </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA75" t="s">
+        <v>796</v>
+      </c>
+      <c r="AB75" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="76" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>266</v>
       </c>
@@ -5757,8 +6837,14 @@
       <c r="Z76" t="s">
         <v>651</v>
       </c>
-    </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA76" t="s">
+        <v>797</v>
+      </c>
+      <c r="AB76" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="77" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>267</v>
       </c>
@@ -5771,8 +6857,14 @@
       <c r="Z77" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA77" t="s">
+        <v>798</v>
+      </c>
+      <c r="AB77" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="78" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>268</v>
       </c>
@@ -5782,8 +6874,14 @@
       <c r="Z78" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA78" t="s">
+        <v>799</v>
+      </c>
+      <c r="AB78" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="79" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>269</v>
       </c>
@@ -5793,8 +6891,14 @@
       <c r="Z79" t="s">
         <v>654</v>
       </c>
-    </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA79" t="s">
+        <v>800</v>
+      </c>
+      <c r="AB79" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="80" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>270</v>
       </c>
@@ -5804,8 +6908,14 @@
       <c r="Z80" t="s">
         <v>655</v>
       </c>
-    </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA80" t="s">
+        <v>801</v>
+      </c>
+      <c r="AB80" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="81" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>271</v>
       </c>
@@ -5815,8 +6925,14 @@
       <c r="Z81" t="s">
         <v>656</v>
       </c>
-    </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA81" t="s">
+        <v>802</v>
+      </c>
+      <c r="AB81" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="82" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>272</v>
       </c>
@@ -5826,8 +6942,14 @@
       <c r="Z82" t="s">
         <v>657</v>
       </c>
-    </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA82" t="s">
+        <v>803</v>
+      </c>
+      <c r="AB82" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="83" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>273</v>
       </c>
@@ -5837,260 +6959,518 @@
       <c r="Z83" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA83" t="s">
+        <v>804</v>
+      </c>
+      <c r="AB83" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="84" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>274</v>
       </c>
       <c r="Z84" t="s">
         <v>659</v>
       </c>
-    </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA84" t="s">
+        <v>805</v>
+      </c>
+      <c r="AB84" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="85" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>275</v>
       </c>
       <c r="Z85" t="s">
         <v>660</v>
       </c>
-    </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA85" t="s">
+        <v>806</v>
+      </c>
+      <c r="AB85" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="86" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>276</v>
       </c>
       <c r="Z86" t="s">
         <v>661</v>
       </c>
-    </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA86" t="s">
+        <v>807</v>
+      </c>
+      <c r="AB86" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="87" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>277</v>
       </c>
       <c r="Z87" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA87" t="s">
+        <v>808</v>
+      </c>
+      <c r="AB87" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="88" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>278</v>
       </c>
       <c r="Z88" t="s">
         <v>663</v>
       </c>
-    </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA88" t="s">
+        <v>809</v>
+      </c>
+      <c r="AB88" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="89" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>279</v>
       </c>
       <c r="Z89" t="s">
         <v>664</v>
       </c>
-    </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA89" t="s">
+        <v>810</v>
+      </c>
+      <c r="AB89" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="90" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>280</v>
       </c>
       <c r="Z90" t="s">
         <v>665</v>
       </c>
-    </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA90" t="s">
+        <v>811</v>
+      </c>
+      <c r="AB90" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="91" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>281</v>
       </c>
       <c r="Z91" t="s">
         <v>666</v>
       </c>
-    </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA91" t="s">
+        <v>812</v>
+      </c>
+      <c r="AB91" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="92" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>282</v>
       </c>
       <c r="Z92" t="s">
         <v>667</v>
       </c>
-    </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA92" t="s">
+        <v>813</v>
+      </c>
+      <c r="AB92" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="93" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>283</v>
       </c>
       <c r="Z93" t="s">
         <v>668</v>
       </c>
-    </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA93" t="s">
+        <v>814</v>
+      </c>
+      <c r="AB93" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="94" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>284</v>
       </c>
       <c r="Z94" t="s">
         <v>669</v>
       </c>
-    </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA94" t="s">
+        <v>815</v>
+      </c>
+      <c r="AB94" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="95" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>285</v>
       </c>
       <c r="Z95" t="s">
         <v>670</v>
       </c>
-    </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA95" t="s">
+        <v>816</v>
+      </c>
+      <c r="AB95" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="96" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>286</v>
       </c>
       <c r="Z96" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA96" t="s">
+        <v>817</v>
+      </c>
+      <c r="AB96" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="97" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>287</v>
       </c>
       <c r="Z97" t="s">
         <v>672</v>
       </c>
-    </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA97" t="s">
+        <v>818</v>
+      </c>
+      <c r="AB97" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="98" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>288</v>
       </c>
       <c r="Z98" t="s">
         <v>673</v>
       </c>
-    </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA98" t="s">
+        <v>819</v>
+      </c>
+      <c r="AB98" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="99" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>289</v>
       </c>
       <c r="Z99" t="s">
         <v>674</v>
       </c>
-    </row>
-    <row r="100" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA99" t="s">
+        <v>820</v>
+      </c>
+      <c r="AB99" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="100" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>290</v>
       </c>
       <c r="Z100" t="s">
         <v>675</v>
       </c>
-    </row>
-    <row r="101" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA100" t="s">
+        <v>821</v>
+      </c>
+      <c r="AB100" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="101" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>291</v>
       </c>
       <c r="Z101" t="s">
         <v>676</v>
       </c>
-    </row>
-    <row r="102" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA101" t="s">
+        <v>822</v>
+      </c>
+      <c r="AB101" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="102" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>292</v>
       </c>
       <c r="Z102" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="103" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA102" t="s">
+        <v>823</v>
+      </c>
+      <c r="AB102" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="103" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>293</v>
       </c>
       <c r="Z103" t="s">
         <v>678</v>
       </c>
-    </row>
-    <row r="104" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA103" t="s">
+        <v>824</v>
+      </c>
+      <c r="AB103" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="104" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>294</v>
       </c>
       <c r="Z104" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="105" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA104" t="s">
+        <v>825</v>
+      </c>
+      <c r="AB104" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="105" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>295</v>
       </c>
       <c r="Z105" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="106" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA105" t="s">
+        <v>826</v>
+      </c>
+      <c r="AB105" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="106" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>296</v>
       </c>
       <c r="Z106" t="s">
         <v>681</v>
       </c>
-    </row>
-    <row r="107" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA106" t="s">
+        <v>827</v>
+      </c>
+      <c r="AB106" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="107" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>297</v>
       </c>
       <c r="Z107" t="s">
         <v>682</v>
       </c>
-    </row>
-    <row r="108" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA107" t="s">
+        <v>828</v>
+      </c>
+      <c r="AB107" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="108" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>298</v>
       </c>
       <c r="Z108" t="s">
         <v>683</v>
       </c>
-    </row>
-    <row r="109" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA108" t="s">
+        <v>829</v>
+      </c>
+      <c r="AB108" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="109" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>299</v>
       </c>
       <c r="Z109" t="s">
         <v>684</v>
       </c>
-    </row>
-    <row r="110" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA109" t="s">
+        <v>830</v>
+      </c>
+      <c r="AB109" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="110" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>300</v>
       </c>
       <c r="Z110" t="s">
         <v>685</v>
       </c>
-    </row>
-    <row r="111" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA110" t="s">
+        <v>831</v>
+      </c>
+      <c r="AB110" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="111" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>301</v>
       </c>
       <c r="Z111" t="s">
         <v>686</v>
       </c>
-    </row>
-    <row r="112" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA111" t="s">
+        <v>832</v>
+      </c>
+      <c r="AB111" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="112" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>302</v>
       </c>
       <c r="Z112" t="s">
         <v>687</v>
       </c>
-    </row>
-    <row r="113" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA112" t="s">
+        <v>833</v>
+      </c>
+      <c r="AB112" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="113" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>303</v>
       </c>
       <c r="Z113" t="s">
         <v>688</v>
       </c>
-    </row>
-    <row r="114" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA113" t="s">
+        <v>834</v>
+      </c>
+      <c r="AB113" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="114" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="115" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA114" t="s">
+        <v>835</v>
+      </c>
+      <c r="AB114" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="115" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="116" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="AA115" t="s">
+        <v>836</v>
+      </c>
+      <c r="AB115" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="116" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>306</v>
+      </c>
+      <c r="AA116" t="s">
+        <v>837</v>
+      </c>
+      <c r="AB116" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="117" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AA117" t="s">
+        <v>838</v>
+      </c>
+      <c r="AB117" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="118" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AA118" t="s">
+        <v>839</v>
+      </c>
+      <c r="AB118" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="119" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AA119" t="s">
+        <v>840</v>
+      </c>
+      <c r="AB119" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="120" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AB120" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="121" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AB121" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="122" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AB122" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="123" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AB123" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="124" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AB124" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="125" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AB125" t="s">
+        <v>948</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Base: remove model2, add clean analysis
</commit_message>
<xml_diff>
--- a/data/vars/combination.xlsx
+++ b/data/vars/combination.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="3" documentId="BFB9858DB2A94ED4886500BB2069F5AEF8034D62" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{967D9710-F1BF-41C8-8D1C-C9CE5A9E4CF6}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="BFB9858DB2A94ED4886500BB2069F5AEF8034D62" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{21978FFA-2D02-4585-95E4-8703EBED5CAC}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21160" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45070,7 +45070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:DJ139"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -64458,8 +64458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4AA4B8C-CE05-4319-A4CE-B66CA4C50D28}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>